<commit_message>
Update presentation based on Azadeh's feedback
</commit_message>
<xml_diff>
--- a/assets/tables/2021-09-06-Tables.xlsx
+++ b/assets/tables/2021-09-06-Tables.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Documents\Thesis\thesis_presentation\assets\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1EA260-DBA3-4001-BFB8-49BD3347AD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF32722-058A-4CF1-8F03-4E450B9F4A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{67A94AEB-F11C-4AB3-B28A-F49A4C301124}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{67A94AEB-F11C-4AB3-B28A-F49A4C301124}"/>
   </bookViews>
   <sheets>
     <sheet name="Significant Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Model Fit" sheetId="2" r:id="rId2"/>
-    <sheet name="Participant Characteristics" sheetId="3" r:id="rId3"/>
-    <sheet name="Participant Characteristics Lon" sheetId="4" r:id="rId4"/>
-    <sheet name="Ttest" sheetId="6" r:id="rId5"/>
-    <sheet name="PCorr" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId3"/>
+    <sheet name="Participant Characteristics" sheetId="3" r:id="rId4"/>
+    <sheet name="Participant Characteristics Lon" sheetId="4" r:id="rId5"/>
+    <sheet name="Ttest" sheetId="6" r:id="rId6"/>
+    <sheet name="PCorr" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="465">
   <si>
     <t>Population</t>
   </si>
@@ -1416,13 +1417,34 @@
   </si>
   <si>
     <t>Intercorrelations between Factors</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>IQ</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Attention</t>
+  </si>
+  <si>
+    <t>Sensory</t>
+  </si>
+  <si>
+    <t>RRBs</t>
+  </si>
+  <si>
+    <t>Social Communication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1478,8 +1500,28 @@
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1558,8 +1600,62 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3F4077"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE77E24"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCE5F57"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF47A5A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDB715"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF60AD45"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF34444F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF125C83"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1612,11 +1708,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1772,6 +1888,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1811,18 +1939,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1851,6 +1979,90 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1861,15 +2073,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF125C83"/>
+      <color rgb="FF34444F"/>
+      <color rgb="FF60AD45"/>
+      <color rgb="FFFDB715"/>
+      <color rgb="FF47A5A2"/>
+      <color rgb="FFCE5F57"/>
+      <color rgb="FFE77E24"/>
+      <color rgb="FF3F4077"/>
+      <color rgb="FF58595B"/>
       <color rgb="FFE25656"/>
-      <color rgb="FF4B7AA9"/>
-      <color rgb="FFFDB816"/>
-      <color rgb="FF58595B"/>
-      <color rgb="FF8798A9"/>
-      <color rgb="FF718DA9"/>
-      <color rgb="FFE29494"/>
-      <color rgb="FFFDE3A7"/>
-      <color rgb="FFFFCCCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2225,10 +2438,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="61" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2251,8 +2464,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2273,8 +2486,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2295,8 +2508,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
@@ -2317,8 +2530,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2339,8 +2552,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2361,8 +2574,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2383,8 +2596,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
@@ -2405,8 +2618,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="58"/>
-      <c r="B10" s="58"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
@@ -2427,8 +2640,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="58"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2449,8 +2662,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="58"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2471,8 +2684,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="58"/>
-      <c r="B13" s="58"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
@@ -2493,8 +2706,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="55" t="s">
+      <c r="A14" s="62"/>
+      <c r="B14" s="59" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -2517,8 +2730,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
@@ -2539,8 +2752,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
@@ -2561,8 +2774,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
@@ -2583,8 +2796,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="59"/>
       <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
@@ -2605,8 +2818,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2627,8 +2840,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="2" t="s">
         <v>23</v>
       </c>
@@ -2649,8 +2862,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2671,8 +2884,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
-      <c r="B22" s="55"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
@@ -2693,8 +2906,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="58"/>
-      <c r="B23" s="59" t="s">
+      <c r="A23" s="62"/>
+      <c r="B23" s="63" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2717,8 +2930,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
-      <c r="B24" s="59"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
@@ -2739,8 +2952,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2761,8 +2974,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2783,10 +2996,10 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="63" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2809,8 +3022,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="59"/>
+      <c r="A28" s="63"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
@@ -2831,8 +3044,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
-      <c r="B29" s="59"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="63"/>
       <c r="C29" s="1" t="s">
         <v>10</v>
       </c>
@@ -2853,8 +3066,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
-      <c r="B30" s="59"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="63"/>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
@@ -2875,8 +3088,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
-      <c r="B31" s="59"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="1" t="s">
         <v>17</v>
       </c>
@@ -2897,8 +3110,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="63"/>
       <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
@@ -2919,8 +3132,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59" t="s">
+      <c r="A33" s="63"/>
+      <c r="B33" s="63" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -2943,8 +3156,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="63"/>
+      <c r="B34" s="63"/>
       <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
@@ -2965,8 +3178,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
-      <c r="B35" s="59"/>
+      <c r="A35" s="63"/>
+      <c r="B35" s="63"/>
       <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
@@ -2987,8 +3200,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="59"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="63"/>
       <c r="C36" s="2" t="s">
         <v>21</v>
       </c>
@@ -3009,8 +3222,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="59"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="63"/>
       <c r="C37" s="1" t="s">
         <v>23</v>
       </c>
@@ -3031,8 +3244,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="59"/>
+      <c r="A38" s="63"/>
+      <c r="B38" s="63"/>
       <c r="C38" s="2" t="s">
         <v>23</v>
       </c>
@@ -3053,8 +3266,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="59"/>
-      <c r="B39" s="59"/>
+      <c r="A39" s="63"/>
+      <c r="B39" s="63"/>
       <c r="C39" s="1" t="s">
         <v>23</v>
       </c>
@@ -3075,8 +3288,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
-      <c r="B40" s="55" t="s">
+      <c r="A40" s="63"/>
+      <c r="B40" s="59" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -3099,8 +3312,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
-      <c r="B41" s="55"/>
+      <c r="A41" s="63"/>
+      <c r="B41" s="59"/>
       <c r="C41" s="1" t="s">
         <v>25</v>
       </c>
@@ -3121,8 +3334,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="59"/>
       <c r="C42" s="2" t="s">
         <v>25</v>
       </c>
@@ -3143,7 +3356,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="59" t="s">
+      <c r="A43" s="63" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3169,8 +3382,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="55" t="s">
+      <c r="A44" s="63"/>
+      <c r="B44" s="59" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -3193,8 +3406,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="63"/>
+      <c r="B45" s="59"/>
       <c r="C45" s="1" t="s">
         <v>23</v>
       </c>
@@ -3215,8 +3428,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
-      <c r="B46" s="55" t="s">
+      <c r="A46" s="63"/>
+      <c r="B46" s="59" t="s">
         <v>24</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -3239,8 +3452,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="55"/>
+      <c r="A47" s="63"/>
+      <c r="B47" s="59"/>
       <c r="C47" s="1" t="s">
         <v>25</v>
       </c>
@@ -3261,8 +3474,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="59"/>
-      <c r="B48" s="55"/>
+      <c r="A48" s="63"/>
+      <c r="B48" s="59"/>
       <c r="C48" s="2" t="s">
         <v>25</v>
       </c>
@@ -3283,8 +3496,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="59"/>
-      <c r="B49" s="55"/>
+      <c r="A49" s="63"/>
+      <c r="B49" s="59"/>
       <c r="C49" s="1" t="s">
         <v>25</v>
       </c>
@@ -3305,7 +3518,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="55" t="s">
+      <c r="A50" s="59" t="s">
         <v>29</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -3331,7 +3544,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="55"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="1" t="s">
         <v>24</v>
       </c>
@@ -3355,7 +3568,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
+      <c r="A52" s="60"/>
       <c r="B52" s="3" t="s">
         <v>24</v>
       </c>
@@ -3402,7 +3615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E99939-21DF-48E1-AB6C-F8CCC5640EA0}">
   <dimension ref="A2:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -3449,7 +3662,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="52" t="s">
@@ -3481,7 +3694,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="50" t="s">
         <v>20</v>
       </c>
@@ -3511,7 +3724,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="53" t="s">
         <v>24</v>
       </c>
@@ -3541,7 +3754,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="66" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="50" t="s">
@@ -3573,7 +3786,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="53" t="s">
         <v>20</v>
       </c>
@@ -3603,7 +3816,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="50" t="s">
         <v>24</v>
       </c>
@@ -3633,7 +3846,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="67" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="53" t="s">
@@ -3665,7 +3878,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="50" t="s">
         <v>20</v>
       </c>
@@ -3695,7 +3908,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="53" t="s">
         <v>24</v>
       </c>
@@ -3725,7 +3938,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="68" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="50" t="s">
@@ -3757,7 +3970,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="53" t="s">
         <v>20</v>
       </c>
@@ -3787,7 +4000,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="65"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="54" t="s">
         <v>24</v>
       </c>
@@ -3829,6 +4042,336 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C045C98C-B146-4A5F-AB5E-1062B855F95C}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="6" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="97" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="109" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="88" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="98"/>
+      <c r="B3" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="109" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="99"/>
+      <c r="B4" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="110" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="90" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="100" t="s">
+        <v>459</v>
+      </c>
+      <c r="B5" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="92" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="91" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="111" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="91" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="92" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
+        <v>460</v>
+      </c>
+      <c r="B7" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="111" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="91" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7" s="92" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="103" t="s">
+        <v>461</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="91" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="91" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" s="92" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="104" t="s">
+        <v>462</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="91" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="111" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="92" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="105" t="s">
+        <v>463</v>
+      </c>
+      <c r="B10" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" s="94" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="106"/>
+      <c r="B11" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="110" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="89" t="s">
+        <v>176</v>
+      </c>
+      <c r="F11" s="90" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="107" t="s">
+        <v>464</v>
+      </c>
+      <c r="B12" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="113" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="95" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="96" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="107"/>
+      <c r="B13" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="95" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="113" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="95" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="96" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="107"/>
+      <c r="B14" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="113" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="96" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="107"/>
+      <c r="B15" s="95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="113" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="95" t="s">
+        <v>180</v>
+      </c>
+      <c r="F15" s="96" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="108"/>
+      <c r="B16" s="89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="89" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="110" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="89" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" s="90" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B76B51-2917-4027-BB6A-8A15D39E82A2}">
   <dimension ref="A1:AF14"/>
   <sheetViews>
@@ -3854,66 +4397,66 @@
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66" t="s">
+      <c r="H1" s="70"/>
+      <c r="I1" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66" t="s">
+      <c r="J1" s="70"/>
+      <c r="K1" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66" t="s">
+      <c r="N1" s="70"/>
+      <c r="O1" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66" t="s">
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66" t="s">
+      <c r="R1" s="70"/>
+      <c r="S1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66" t="s">
+      <c r="T1" s="70"/>
+      <c r="U1" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66" t="s">
+      <c r="V1" s="70"/>
+      <c r="W1" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66" t="s">
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66" t="s">
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66" t="s">
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66" t="s">
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="66"/>
+      <c r="AF1" s="70"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -4014,7 +4557,7 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="70" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -4112,7 +4655,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="10" t="s">
         <v>60</v>
       </c>
@@ -4208,7 +4751,7 @@
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="10" t="s">
         <v>76</v>
       </c>
@@ -4304,7 +4847,7 @@
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="70" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -4402,7 +4945,7 @@
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="10" t="s">
         <v>60</v>
       </c>
@@ -4498,7 +5041,7 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="10" t="s">
         <v>76</v>
       </c>
@@ -4594,7 +5137,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="70" t="s">
         <v>137</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -4692,7 +5235,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="10" t="s">
         <v>60</v>
       </c>
@@ -4788,7 +5331,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="10" t="s">
         <v>76</v>
       </c>
@@ -4884,7 +5427,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="70" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -4982,7 +5525,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="10" t="s">
         <v>60</v>
       </c>
@@ -5078,7 +5621,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="11" t="s">
         <v>76</v>
       </c>
@@ -5175,6 +5718,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="AA1:AB1"/>
@@ -5191,15 +5737,12 @@
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9C7552-9812-4D5B-8A82-1CCD801D489C}">
   <dimension ref="A1:N41"/>
   <sheetViews>
@@ -5215,22 +5758,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="41"/>
@@ -5240,26 +5783,26 @@
       <c r="B3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73" t="s">
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="74" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="75" t="s">
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
     </row>
     <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -5304,7 +5847,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="72" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -5348,7 +5891,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="18" t="s">
         <v>42</v>
       </c>
@@ -5390,7 +5933,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="72" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -5434,7 +5977,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
+      <c r="A8" s="73"/>
       <c r="B8" s="18" t="s">
         <v>42</v>
       </c>
@@ -5476,7 +6019,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="72" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -5520,7 +6063,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
+      <c r="A10" s="73"/>
       <c r="B10" s="18" t="s">
         <v>42</v>
       </c>
@@ -5562,7 +6105,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="72" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -5606,7 +6149,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="18" t="s">
         <v>42</v>
       </c>
@@ -5648,7 +6191,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -5692,7 +6235,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
+      <c r="A14" s="73"/>
       <c r="B14" s="18" t="s">
         <v>42</v>
       </c>
@@ -5734,7 +6277,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="72" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -5778,7 +6321,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="18" t="s">
         <v>42</v>
       </c>
@@ -5820,7 +6363,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="72" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -5864,7 +6407,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="18" t="s">
         <v>42</v>
       </c>
@@ -5906,7 +6449,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -5950,7 +6493,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
+      <c r="A20" s="73"/>
       <c r="B20" s="18" t="s">
         <v>42</v>
       </c>
@@ -5992,7 +6535,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="72" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -6036,7 +6579,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="18" t="s">
         <v>42</v>
       </c>
@@ -6078,7 +6621,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="72" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -6122,7 +6665,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
+      <c r="A24" s="73"/>
       <c r="B24" s="18" t="s">
         <v>42</v>
       </c>
@@ -6164,7 +6707,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="69" t="s">
+      <c r="A25" s="72" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -6208,7 +6751,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
+      <c r="A26" s="73"/>
       <c r="B26" s="18" t="s">
         <v>42</v>
       </c>
@@ -6250,7 +6793,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="72" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -6294,7 +6837,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="71"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="18" t="s">
         <v>42</v>
       </c>
@@ -6336,7 +6879,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="72" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="13" t="s">
@@ -6380,7 +6923,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="71"/>
+      <c r="A30" s="73"/>
       <c r="B30" s="18" t="s">
         <v>42</v>
       </c>
@@ -6422,7 +6965,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="72" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="13" t="s">
@@ -6466,7 +7009,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="71"/>
+      <c r="A32" s="73"/>
       <c r="B32" s="18" t="s">
         <v>42</v>
       </c>
@@ -6508,7 +7051,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="72" t="s">
         <v>40</v>
       </c>
       <c r="B33" s="13" t="s">
@@ -6552,7 +7095,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="70"/>
+      <c r="A34" s="75"/>
       <c r="B34" s="14" t="s">
         <v>42</v>
       </c>
@@ -6601,18 +7144,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:H3"/>
@@ -6621,6 +7152,18 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6630,7 +7173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACAEB54-38B6-4D26-A3F2-5A9F9A2408BC}">
   <dimension ref="A1:J16"/>
   <sheetViews>
@@ -6646,18 +7189,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="74" t="s">
         <v>437</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="43"/>
@@ -6703,7 +7246,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="80" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="46" t="s">
@@ -6735,7 +7278,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="46" t="s">
         <v>17</v>
       </c>
@@ -6765,7 +7308,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="46" t="s">
         <v>21</v>
       </c>
@@ -6795,7 +7338,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="46" t="s">
         <v>23</v>
       </c>
@@ -6825,7 +7368,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="48" t="s">
         <v>25</v>
       </c>
@@ -6855,7 +7398,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="83" t="s">
         <v>422</v>
       </c>
       <c r="B9" s="46" t="s">
@@ -6887,7 +7430,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="46" t="s">
         <v>17</v>
       </c>
@@ -6917,7 +7460,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="46" t="s">
         <v>21</v>
       </c>
@@ -6947,7 +7490,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="46" t="s">
         <v>23</v>
       </c>
@@ -6977,7 +7520,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="80"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="49" t="s">
         <v>25</v>
       </c>
@@ -7022,7 +7565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0067618-65A0-426E-BFC5-BE1E689FD660}">
   <dimension ref="A1:P18"/>
   <sheetViews>
@@ -7036,24 +7579,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="85" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="42"/>

</xml_diff>